<commit_message>
inicio de la lectura al precálculo de stewart sección 1.2 potenciación y radicación
</commit_message>
<xml_diff>
--- a/evaluation/calificaciones_diferencial.xlsx
+++ b/evaluation/calificaciones_diferencial.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Email</t>
   </si>
   <si>
-    <t xml:space="preserve">Task₁</t>
+    <t xml:space="preserve">Task₁ excel funcion lineal</t>
   </si>
   <si>
     <t xml:space="preserve">Task₂ Horario</t>
@@ -311,11 +311,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -339,7 +339,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,7 +528,9 @@
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="D14" s="2" t="n">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
agosto 25 de 2023
</commit_message>
<xml_diff>
--- a/evaluation/calificaciones_diferencial.xlsx
+++ b/evaluation/calificaciones_diferencial.xlsx
@@ -339,7 +339,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,7 +534,9 @@
       <c r="D14" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
@@ -650,8 +652,12 @@
       <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>

</xml_diff>

<commit_message>
notas del primer parcial listas
</commit_message>
<xml_diff>
--- a/evaluation/calificaciones_diferencial.xlsx
+++ b/evaluation/calificaciones_diferencial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Task₂ Horario</t>
   </si>
   <si>
-    <t xml:space="preserve">Task₃</t>
+    <t xml:space="preserve">Task₃ Parcial 1</t>
   </si>
   <si>
     <t xml:space="preserve">AGUDELO MORENO RENATO DIRNEY</t>
@@ -73,6 +73,9 @@
     <t xml:space="preserve">paula.bula@udea.edu.co</t>
   </si>
   <si>
+    <t xml:space="preserve">2.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">CANTILLO ENSUCHO DANIEL</t>
   </si>
   <si>
@@ -163,6 +166,9 @@
     <t xml:space="preserve">erlinda.perez@udea.edu.co</t>
   </si>
   <si>
+    <t xml:space="preserve">3.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">PINEDA ROMERO YOSMERI</t>
   </si>
   <si>
@@ -173,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve">mariana.quinonezc@udea.edu.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3</t>
   </si>
   <si>
     <t xml:space="preserve">QUIROZ DURAN JUAN MANUEL</t>
@@ -339,7 +348,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -374,7 +383,9 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
@@ -387,7 +398,9 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -400,7 +413,9 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
@@ -413,7 +428,9 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
@@ -426,7 +443,9 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
@@ -439,94 +458,108 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>5</v>
@@ -542,115 +575,131 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>5</v>
@@ -658,124 +707,146 @@
       <c r="D23" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>

</xml_diff>

<commit_message>
notas de las dos primeras tareas
</commit_message>
<xml_diff>
--- a/evaluation/calificaciones_diferencial.xlsx
+++ b/evaluation/calificaciones_diferencial.xlsx
@@ -311,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,6 +326,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -348,13 +352,15 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="66.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,8 +387,12 @@
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E2" s="2" t="n">
         <v>5</v>
       </c>
@@ -396,8 +406,12 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E3" s="2" t="n">
         <v>5</v>
       </c>
@@ -599,8 +613,12 @@
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E16" s="2" t="n">
         <v>5</v>
       </c>
@@ -614,8 +632,12 @@
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="C17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E17" s="2" t="n">
         <v>5</v>
       </c>
@@ -629,8 +651,12 @@
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E18" s="2" t="n">
         <v>5</v>
       </c>
@@ -645,8 +671,12 @@
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="C19" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E19" s="2" t="n">
         <v>5</v>
       </c>
@@ -660,8 +690,12 @@
       <c r="B20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E20" s="2" t="n">
         <v>5</v>
       </c>
@@ -675,8 +709,12 @@
       <c r="B21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E21" s="2" t="n">
         <v>5</v>
       </c>
@@ -690,8 +728,12 @@
       <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E22" s="2" t="s">
         <v>48</v>
       </c>
@@ -724,7 +766,9 @@
       <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="D24" s="2" t="n">
         <v>5</v>
       </c>
@@ -741,8 +785,12 @@
       <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E25" s="2" t="n">
         <v>5</v>
       </c>
@@ -756,8 +804,12 @@
       <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E26" s="2" t="n">
         <v>5</v>
       </c>
@@ -771,8 +823,12 @@
       <c r="B27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="C27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E27" s="2" t="n">
         <v>5</v>
       </c>
@@ -786,8 +842,12 @@
       <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="C28" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E28" s="2" t="n">
         <v>5</v>
       </c>
@@ -801,8 +861,12 @@
       <c r="B29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="C29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E29" s="2" t="n">
         <v>5</v>
       </c>
@@ -816,8 +880,12 @@
       <c r="B30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="C30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E30" s="2" t="n">
         <v>5</v>
       </c>
@@ -831,7 +899,9 @@
       <c r="B31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="n">
         <v>5</v>
@@ -846,8 +916,12 @@
       <c r="B32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="C32" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E32" s="2" t="n">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
carpeta para la enseñanza de la función exponencial
</commit_message>
<xml_diff>
--- a/evaluation/calificaciones_diferencial.xlsx
+++ b/evaluation/calificaciones_diferencial.xlsx
@@ -352,7 +352,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,8 +425,12 @@
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E4" s="2" t="n">
         <v>5</v>
       </c>
@@ -459,8 +463,12 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E6" s="2" t="n">
         <v>5</v>
       </c>
@@ -474,8 +482,12 @@
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
@@ -489,8 +501,12 @@
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E8" s="2" t="n">
         <v>5</v>
       </c>
@@ -504,8 +520,12 @@
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E9" s="2" t="n">
         <v>5</v>
       </c>
@@ -519,8 +539,12 @@
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E10" s="2" t="n">
         <v>5</v>
       </c>
@@ -534,8 +558,12 @@
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E11" s="2" t="n">
         <v>5</v>
       </c>
@@ -549,8 +577,12 @@
       <c r="B12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E12" s="2" t="n">
         <v>5</v>
       </c>
@@ -564,8 +596,12 @@
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E13" s="2" t="n">
         <v>5</v>
       </c>
@@ -598,8 +634,12 @@
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="E15" s="2" t="n">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Inicio de la interpretación de la pendiente de una recta como razón constante de cambio o velocidad de cambio
</commit_message>
<xml_diff>
--- a/evaluation/calificaciones_diferencial.xlsx
+++ b/evaluation/calificaciones_diferencial.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">Task₃ Parcial 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Tarea 4 visualizacion de funciones en excel con video</t>
+  </si>
+  <si>
     <t xml:space="preserve">AGUDELO MORENO RENATO DIRNEY</t>
   </si>
   <si>
@@ -112,7 +115,7 @@
     <t xml:space="preserve">camilo.humanez@udea.edu.co</t>
   </si>
   <si>
-    <t xml:space="preserve">IBAnEZ MORENO FRANCISCO LUIS</t>
+    <t xml:space="preserve">IBAÑEZ MORENO FRANCISCO LUIS</t>
   </si>
   <si>
     <t xml:space="preserve">francisco.ibanez@udea.edu.co</t>
@@ -344,6 +347,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -352,15 +461,17 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="66.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -379,13 +490,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>0</v>
@@ -401,10 +515,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
@@ -420,10 +534,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>5</v>
@@ -439,10 +553,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>5</v>
@@ -458,10 +572,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>5</v>
@@ -477,10 +591,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>5</v>
@@ -489,17 +603,17 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>5</v>
@@ -515,10 +629,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>5</v>
@@ -534,10 +648,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
@@ -553,10 +667,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>5</v>
@@ -572,10 +686,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
@@ -591,10 +705,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>3</v>
@@ -610,10 +724,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>5</v>
@@ -629,10 +743,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>0</v>
@@ -648,10 +762,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
@@ -667,10 +781,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
@@ -686,10 +800,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
@@ -706,10 +820,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>5</v>
@@ -725,10 +839,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>5</v>
@@ -744,10 +858,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
@@ -763,10 +877,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
@@ -775,17 +889,17 @@
         <v>0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>5</v>
@@ -801,10 +915,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>5</v>
@@ -813,17 +927,17 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>0</v>
@@ -839,10 +953,10 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>5</v>
@@ -858,10 +972,10 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0</v>
@@ -877,10 +991,10 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>5</v>
@@ -896,10 +1010,10 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>0</v>
@@ -915,10 +1029,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>0</v>
@@ -934,15 +1048,17 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="n">
+        <v>5</v>
+      </c>
       <c r="E31" s="2" t="n">
         <v>5</v>
       </c>
@@ -951,10 +1067,10 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>5</v>

</xml_diff>